<commit_message>
Remove unnecessary interrupt handling.  Add stats reporting so that we can see what's happening without having to connect USB interface.  Correct the sense of the "GPS on" pin.  Increase accelerometer threshold slightly.  Finalised PCB and BoM.
</commit_message>
<xml_diff>
--- a/hardware/bom.xlsx
+++ b/hardware/bom.xlsx
@@ -84,9 +84,6 @@
     <t>FET</t>
   </si>
   <si>
-    <t>FQPF27P06</t>
-  </si>
-  <si>
     <t>Fairchild</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
   </si>
   <si>
     <t>ADXL345 breakout board</t>
-  </si>
-  <si>
-    <t>http://uk.rs-online.com/web/p/mosfet-transistors/8075901</t>
   </si>
   <si>
     <t>http://uk.rs-online.com/web/p/through-hole-fixed-resistors/7077745/</t>
@@ -302,6 +296,12 @@
   <si>
     <t>Notes</t>
   </si>
+  <si>
+    <t>NDP6020P</t>
+  </si>
+  <si>
+    <t>http://uk.rs-online.com/web/p/mosfet-transistors/8061230/</t>
+  </si>
 </sst>
 </file>
 
@@ -468,7 +468,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -579,6 +579,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="52" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -973,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q884"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="162" zoomScalePageLayoutView="162" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="111" zoomScaleNormal="162" zoomScalePageLayoutView="162" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -1000,7 +1003,7 @@
   <sheetData>
     <row r="1" spans="2:17">
       <c r="B1" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="2:17">
@@ -1021,22 +1024,22 @@
     </row>
     <row r="3" spans="2:17" s="5" customFormat="1" ht="25.5">
       <c r="B3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="22" t="s">
         <v>9</v>
@@ -1066,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:17">
@@ -1099,7 +1102,7 @@
       <c r="O4" s="32"/>
       <c r="P4" s="33"/>
       <c r="Q4" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:17">
@@ -1107,7 +1110,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="28" t="str">
         <f>"---"</f>
@@ -1134,7 +1137,7 @@
       <c r="O5" s="32"/>
       <c r="P5" s="33"/>
       <c r="Q5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:17">
@@ -1142,7 +1145,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="28" t="str">
         <f>"---"</f>
@@ -1155,7 +1158,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="29" t="s">
         <v>10</v>
@@ -1169,7 +1172,7 @@
       <c r="O6" s="32"/>
       <c r="P6" s="33"/>
       <c r="Q6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:17">
@@ -1177,7 +1180,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" s="28" t="str">
         <f>"---"</f>
@@ -1187,10 +1190,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="H7" s="29" t="s">
         <v>10</v>
@@ -1203,8 +1206,8 @@
       <c r="N7" s="29"/>
       <c r="O7" s="32"/>
       <c r="P7" s="33"/>
-      <c r="Q7" s="2" t="s">
-        <v>33</v>
+      <c r="Q7" s="39" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:17">
@@ -1212,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="30">
         <v>1</v>
@@ -1240,7 +1243,7 @@
       <c r="O8" s="32"/>
       <c r="P8" s="33"/>
       <c r="Q8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -1248,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="28" t="str">
         <f>"---"</f>
@@ -1258,10 +1261,10 @@
         <v>2</v>
       </c>
       <c r="F9" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="28" t="s">
         <v>22</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>23</v>
       </c>
       <c r="H9" s="29" t="s">
         <v>10</v>
@@ -1275,7 +1278,7 @@
       <c r="O9" s="32"/>
       <c r="P9" s="33"/>
       <c r="Q9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:17">
@@ -1283,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="28" t="str">
         <f>"---"</f>
@@ -1293,10 +1296,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>10</v>
@@ -1310,7 +1313,7 @@
       <c r="O10" s="32"/>
       <c r="P10" s="33"/>
       <c r="Q10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:17">
@@ -1318,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="28" t="str">
         <f t="shared" ref="D11:D16" si="0">"---"</f>
@@ -1328,10 +1331,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>10</v>
@@ -1345,7 +1348,7 @@
       <c r="O11" s="32"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:17">
@@ -1353,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1363,10 +1366,10 @@
         <v>2</v>
       </c>
       <c r="F12" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="29" t="s">
         <v>79</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>81</v>
       </c>
       <c r="H12" s="29"/>
       <c r="I12" s="31"/>
@@ -1378,7 +1381,7 @@
       <c r="O12" s="32"/>
       <c r="P12" s="33"/>
       <c r="Q12" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:17">
@@ -1386,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1396,10 +1399,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>10</v>
@@ -1413,7 +1416,7 @@
       <c r="O13" s="32"/>
       <c r="P13" s="33"/>
       <c r="Q13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="25.5">
@@ -1421,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="28" t="str">
         <f>"---"</f>
@@ -1431,10 +1434,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>76</v>
       </c>
       <c r="H14" s="29"/>
       <c r="I14" s="31"/>
@@ -1446,15 +1449,15 @@
       <c r="O14" s="32"/>
       <c r="P14" s="33"/>
       <c r="Q14" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1464,10 +1467,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="31"/>
@@ -1479,28 +1482,28 @@
       <c r="O15" s="32"/>
       <c r="P15" s="33"/>
       <c r="Q15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:17">
       <c r="B16" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D16" s="28" t="str">
         <f t="shared" si="0"/>
         <v>---</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="31"/>
@@ -1512,12 +1515,12 @@
       <c r="O16" s="32"/>
       <c r="P16" s="33"/>
       <c r="Q16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:17">
       <c r="B18" s="35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1551,22 +1554,22 @@
     </row>
     <row r="20" spans="2:17" s="5" customFormat="1" ht="25.5">
       <c r="B20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="E20" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>31</v>
-      </c>
       <c r="F20" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H20" s="22" t="s">
         <v>9</v>
@@ -1596,28 +1599,28 @@
         <v>4</v>
       </c>
       <c r="Q20" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21" s="28" t="str">
         <f>"---"</f>
         <v>---</v>
       </c>
       <c r="E21" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>10</v>
@@ -1631,7 +1634,7 @@
       <c r="O21" s="32"/>
       <c r="P21" s="33"/>
       <c r="Q21" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:17">
@@ -1639,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D22" s="28" t="str">
         <f>"---"</f>
@@ -1649,10 +1652,10 @@
         <v>2</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>10</v>
@@ -1666,7 +1669,7 @@
       <c r="O22" s="32"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:17">
@@ -1674,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D23" s="28" t="str">
         <f t="shared" ref="D23:D24" si="1">"---"</f>
@@ -1684,10 +1687,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>10</v>
@@ -1701,7 +1704,7 @@
       <c r="O23" s="32"/>
       <c r="P23" s="33"/>
       <c r="Q23" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:17">
@@ -1709,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D24" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1719,10 +1722,10 @@
         <v>1</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>10</v>
@@ -1736,7 +1739,7 @@
       <c r="O24" s="32"/>
       <c r="P24" s="33"/>
       <c r="Q24" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:17">
@@ -15540,42 +15543,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change FET name to correct one (now NDP6020P, not FQPF27P06).  Update BoM.  Add assembly guide.
</commit_message>
<xml_diff>
--- a/hardware/bom.xlsx
+++ b/hardware/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="101">
   <si>
     <t>RESISTOR</t>
   </si>
@@ -222,22 +222,7 @@
     <t>GPS module with built-in antenna</t>
   </si>
   <si>
-    <t>PCB header, JST PH B2B series, 2mm pitch, 2 way, 1 row, through hole</t>
-  </si>
-  <si>
     <t>ABS enclosure, IP54, 121 x 66 x 37 mm</t>
-  </si>
-  <si>
-    <t>3.7V Li-Po rechargeable battery, 2000 mAh, wire lead terminal</t>
-  </si>
-  <si>
-    <t>PCB socket, 0.1" pitch, 19 contacts, 1 row,  through hole</t>
-  </si>
-  <si>
-    <t>PCB socket, 0.1" pitch, 8 contacts, 1 row,  through hole</t>
-  </si>
-  <si>
-    <t>PCB socket, 0.1" pitch, 10 contacts, 1 row,  through hole</t>
   </si>
   <si>
     <t>PCB header, 0.1" pitch, N way (you will need only one from the break-off strip), 1 row, through hole</t>
@@ -302,6 +287,48 @@
   <si>
     <t>http://uk.rs-online.com/web/p/mosfet-transistors/8061230/</t>
   </si>
+  <si>
+    <t>http://uk.rs-online.com/web/p/pcb-connector-housings/8201611/</t>
+  </si>
+  <si>
+    <t>XHP-2</t>
+  </si>
+  <si>
+    <t>PKCell</t>
+  </si>
+  <si>
+    <t>LP103450</t>
+  </si>
+  <si>
+    <t>3.7V Li-Po rechargeable battery, 2000 mAh, wire lead terminal [NOTE 2]</t>
+  </si>
+  <si>
+    <t>Li-Po Battery with JST PH Series 2-pin B2B connector (2 mm pitch), 3.7 V, 2000 mAh dimensions 51 mm x 34 mm x 11.3 mm [NOTE 1]</t>
+  </si>
+  <si>
+    <t>PCB header, JST XH B2B series, 2.5 mm pitch, 2 way, 1 row, through hole [NOTE 3]</t>
+  </si>
+  <si>
+    <t>PCB header, JST PH B2B series, 2 mm pitch, 2 way, 1 row, through hole</t>
+  </si>
+  <si>
+    <t>PCB socket, 0.1" pitch, 1 contact, 1 row,  through hole [NOTE 4]</t>
+  </si>
+  <si>
+    <t>PCB socket, 0.1" pitch, 19 contacts, 1 row,  through hole [NOTE 5]</t>
+  </si>
+  <si>
+    <t>PCB socket, 0.1" pitch, 8 contacts, 1 row,  through hole [NOTE 5]</t>
+  </si>
+  <si>
+    <t>PCB socket, 0.1" pitch, 10 contacts, 1 row,  through hole [NOTE 5]</t>
+  </si>
+  <si>
+    <t>http://uk.rs-online.com/web/p/pcb-headers/8632706/</t>
+  </si>
+  <si>
+    <t>68000-401HLF</t>
+  </si>
 </sst>
 </file>
 
@@ -310,7 +337,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -361,6 +388,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -468,7 +501,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -583,6 +616,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="52" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -650,6 +698,132 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>368986</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>111554</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>4445000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>51487</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="514864" y="5165811"/>
+          <a:ext cx="14338987" cy="1896419"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Notes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>1.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>  This is the battery supplied with the Particle Electron kit.  The PCB is designed such that two batteries can be mounted via a pair of separate connectors on the PCB itself (so the connector on the Electron board is not used and instead the "LiPo" pin on the Electron board is populated with an extra pin during assembly).  These batteries appear to only be available direct from the manufacturer in China.  Hence...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>2.  This is an alternative</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> battery of the same capacity (though physically larger in size) and is available from suppliers in Europe. PLEASE NOTE THAT IF YOU CHOSE TO USE THIS BATTERY YOU MUST USE TWO OF THEM AND DISCARD THE BATTERY THAT CAME WITH THE ELECTON BOARD.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>NEVER</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> MIX BATTERY TYPES AS THIS MAY RESULT IN OVERHEATING/MELTDOWN/FIRE.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>3.  If you chose to us the alternative battery then you will need to use this connector instead of the JST PH B2B series connector and you will  need to modify the PCB design to accept a connector with 2.5 mm pitch pins instead of 2 mm pitch pins (it does also "bodge" into position, just).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>4.  This is the single pin that you solder into the "LiPo" pin of the Electron board if you are fitting a pair of batteries via the connectors on the PCB.  You can, of course, just break off one pin from a larger set of pins.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>5.  The PCB design includes provision for these additional headers.  Fit them if you anticipate a need to probe or connect to the pins.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -974,17 +1148,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q884"/>
+  <dimension ref="B1:Q887"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="111" zoomScaleNormal="162" zoomScalePageLayoutView="162" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="2.140625" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="79.42578125" style="6" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" bestFit="1" customWidth="1"/>
@@ -1003,7 +1177,7 @@
   <sheetData>
     <row r="1" spans="2:17">
       <c r="B1" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="2:17">
@@ -1193,7 +1367,7 @@
         <v>19</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H7" s="29" t="s">
         <v>10</v>
@@ -1207,7 +1381,7 @@
       <c r="O7" s="32"/>
       <c r="P7" s="33"/>
       <c r="Q7" s="39" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:17">
@@ -1251,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="D9" s="28" t="str">
         <f>"---"</f>
@@ -1356,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D12" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1366,10 +1540,10 @@
         <v>2</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H12" s="29"/>
       <c r="I12" s="31"/>
@@ -1381,7 +1555,7 @@
       <c r="O12" s="32"/>
       <c r="P12" s="33"/>
       <c r="Q12" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:17">
@@ -1424,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D14" s="28" t="str">
         <f>"---"</f>
@@ -1434,10 +1608,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H14" s="29"/>
       <c r="I14" s="31"/>
@@ -1449,7 +1623,7 @@
       <c r="O14" s="32"/>
       <c r="P14" s="33"/>
       <c r="Q14" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:17">
@@ -1457,7 +1631,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1490,14 +1664,14 @@
         <v>56</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D16" s="28" t="str">
         <f t="shared" si="0"/>
         <v>---</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>54</v>
@@ -1602,47 +1776,43 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:17">
-      <c r="B21" s="28" t="s">
+    <row r="21" spans="2:17" ht="25.5">
+      <c r="B21" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>67</v>
+      <c r="C21" s="41" t="s">
+        <v>92</v>
       </c>
       <c r="D21" s="28" t="str">
         <f>"---"</f>
         <v>---</v>
       </c>
-      <c r="E21" s="30">
-        <v>2</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>50</v>
+      <c r="E21" s="42">
+        <v>1</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>89</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="31"/>
-      <c r="J21" s="29"/>
+        <v>90</v>
+      </c>
+      <c r="H21" s="29"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="44"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
       <c r="O21" s="32"/>
       <c r="P21" s="33"/>
-      <c r="Q21" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="Q21" s="31"/>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="28" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="D22" s="28" t="str">
         <f>"---"</f>
@@ -1651,11 +1821,11 @@
       <c r="E22" s="30">
         <v>2</v>
       </c>
-      <c r="F22" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>37</v>
+      <c r="F22" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>49</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>10</v>
@@ -1669,7 +1839,7 @@
       <c r="O22" s="32"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:17">
@@ -1677,24 +1847,22 @@
         <v>1</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="D23" s="28" t="str">
-        <f t="shared" ref="D23:D24" si="1">"---"</f>
+        <f>"---"</f>
         <v>---</v>
       </c>
       <c r="E23" s="30">
-        <v>1</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>10</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="29"/>
       <c r="I23" s="31"/>
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
@@ -1703,8 +1871,8 @@
       <c r="N23" s="29"/>
       <c r="O23" s="32"/>
       <c r="P23" s="33"/>
-      <c r="Q23" s="2" t="s">
-        <v>39</v>
+      <c r="Q23" s="39" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="2:17">
@@ -1712,24 +1880,22 @@
         <v>1</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D24" s="28" t="str">
-        <f t="shared" si="1"/>
+        <f>"---"</f>
         <v>---</v>
       </c>
       <c r="E24" s="30">
         <v>1</v>
       </c>
-      <c r="F24" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="H24" s="29" t="s">
-        <v>10</v>
-      </c>
+      <c r="F24" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="29"/>
       <c r="I24" s="31"/>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
@@ -1738,57 +1904,114 @@
       <c r="N24" s="29"/>
       <c r="O24" s="32"/>
       <c r="P24" s="33"/>
-      <c r="Q24" s="2" t="s">
+      <c r="Q24" s="39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17">
+      <c r="B25" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="28" t="str">
+        <f>"---"</f>
+        <v>---</v>
+      </c>
+      <c r="E25" s="30">
+        <v>2</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="31"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17">
+      <c r="B26" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="28" t="str">
+        <f t="shared" ref="D26:D27" si="1">"---"</f>
+        <v>---</v>
+      </c>
+      <c r="E26" s="30">
+        <v>1</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="31"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17">
+      <c r="B27" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>---</v>
+      </c>
+      <c r="E27" s="30">
+        <v>1</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="2:17">
-      <c r="B25" s="1"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-    </row>
-    <row r="26" spans="2:17">
-      <c r="B26" s="1"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-    </row>
-    <row r="27" spans="2:17">
-      <c r="B27" s="1"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="1"/>
@@ -15501,6 +15724,54 @@
       <c r="M884" s="17"/>
       <c r="N884" s="17"/>
       <c r="O884" s="17"/>
+    </row>
+    <row r="885" spans="2:15">
+      <c r="B885" s="1"/>
+      <c r="C885" s="13"/>
+      <c r="D885" s="1"/>
+      <c r="E885" s="14"/>
+      <c r="F885" s="1"/>
+      <c r="G885" s="15"/>
+      <c r="H885" s="16"/>
+      <c r="I885" s="16"/>
+      <c r="J885" s="16"/>
+      <c r="K885" s="16"/>
+      <c r="L885" s="16"/>
+      <c r="M885" s="17"/>
+      <c r="N885" s="17"/>
+      <c r="O885" s="17"/>
+    </row>
+    <row r="886" spans="2:15">
+      <c r="B886" s="1"/>
+      <c r="C886" s="13"/>
+      <c r="D886" s="1"/>
+      <c r="E886" s="14"/>
+      <c r="F886" s="1"/>
+      <c r="G886" s="15"/>
+      <c r="H886" s="16"/>
+      <c r="I886" s="16"/>
+      <c r="J886" s="16"/>
+      <c r="K886" s="16"/>
+      <c r="L886" s="16"/>
+      <c r="M886" s="17"/>
+      <c r="N886" s="17"/>
+      <c r="O886" s="17"/>
+    </row>
+    <row r="887" spans="2:15">
+      <c r="B887" s="1"/>
+      <c r="C887" s="13"/>
+      <c r="D887" s="1"/>
+      <c r="E887" s="14"/>
+      <c r="F887" s="1"/>
+      <c r="G887" s="15"/>
+      <c r="H887" s="16"/>
+      <c r="I887" s="16"/>
+      <c r="J887" s="16"/>
+      <c r="K887" s="16"/>
+      <c r="L887" s="16"/>
+      <c r="M887" s="17"/>
+      <c r="N887" s="17"/>
+      <c r="O887" s="17"/>
     </row>
   </sheetData>
   <sortState ref="B61:M67">
@@ -15518,16 +15789,19 @@
     <hyperlink ref="Q10" r:id="rId7"/>
     <hyperlink ref="Q11" r:id="rId8"/>
     <hyperlink ref="Q13" r:id="rId9"/>
-    <hyperlink ref="Q21" r:id="rId10"/>
-    <hyperlink ref="Q23" r:id="rId11"/>
-    <hyperlink ref="Q24" r:id="rId12"/>
+    <hyperlink ref="Q22" r:id="rId10"/>
+    <hyperlink ref="Q26" r:id="rId11"/>
+    <hyperlink ref="Q27" r:id="rId12"/>
     <hyperlink ref="Q15" r:id="rId13"/>
     <hyperlink ref="Q16" r:id="rId14"/>
     <hyperlink ref="Q14" r:id="rId15"/>
     <hyperlink ref="Q12" r:id="rId16"/>
+    <hyperlink ref="Q23" r:id="rId17"/>
+    <hyperlink ref="Q24" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -15543,42 +15817,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>